<commit_message>
Client's remarks update. Total data updated.
Added finance details for each company.
Added date time for each graphique.
Changed all english interface to franch.
</commit_message>
<xml_diff>
--- a/data/Airbus.xlsx
+++ b/data/Airbus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\extSD\gitRes\StockChooser\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Python\StockChooser\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="17 02 2017" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="14 03 2017" sheetId="18" r:id="rId18"/>
     <sheet name="15 03 2017" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -342,7 +342,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -354,6 +354,7 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -408,6 +409,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -429,12 +436,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -445,7 +467,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -476,6 +498,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -863,20 +888,20 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="101.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" customWidth="1"/>
-    <col min="8" max="17" width="7.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="101.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="17" width="7.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -937,7 +962,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.11865000000000003</v>
+        <v>9.0950000000000031E-2</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1008,11 +1033,11 @@
       </c>
       <c r="C4" s="1">
         <f>D25</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1046,11 +1071,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.88</v>
+        <v>-0.99</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-0.14960000000000001</v>
+        <v>-0.16830000000000001</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1507,7 +1532,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -1545,19 +1570,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -1584,19 +1609,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -1623,19 +1648,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -1662,19 +1687,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -1701,19 +1726,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -1746,7 +1771,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1782,21 +1807,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="66.6328125" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="66.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -1857,7 +1882,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.36499999999999999</v>
+        <v>0.23490000000000003</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1928,11 +1953,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>0.1125</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1966,11 +1991,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.35</v>
+        <v>-0.23</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>5.9499999999999997E-2</v>
+        <v>-3.9100000000000003E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2424,7 +2449,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -2462,19 +2487,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.2</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -2501,19 +2526,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -2540,19 +2565,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -2579,19 +2604,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -2618,19 +2643,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -2669,20 +2694,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -2744,7 +2769,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.27330000000000004</v>
+        <v>0.22990000000000002</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2815,11 +2840,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>0.1125</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2853,11 +2878,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.16</v>
+        <v>-0.23</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-2.7200000000000002E-2</v>
+        <v>-3.9100000000000003E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3311,7 +3336,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -3349,19 +3374,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.2</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -3388,19 +3413,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -3427,19 +3452,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -3466,19 +3491,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -3505,19 +3530,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -3556,21 +3581,21 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="91.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="19" width="14.7265625" customWidth="1"/>
-    <col min="20" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="91.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="19" width="14.7109375" customWidth="1"/>
+    <col min="20" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -3631,7 +3656,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>3.0950000000000005E-2</v>
+        <v>0.28885000000000005</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3702,11 +3727,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -3740,11 +3765,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.89</v>
+        <v>0.68</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-0.15130000000000002</v>
+        <v>0.11560000000000002</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4200,7 +4225,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -4238,19 +4263,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -4277,19 +4302,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -4316,19 +4341,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -4355,19 +4380,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -4394,19 +4419,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -4445,20 +4470,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="102.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="102.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -4519,7 +4544,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.31510000000000005</v>
+        <v>0.36560000000000004</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4590,11 +4615,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -4628,11 +4653,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.27</v>
+        <v>0.08</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-4.5900000000000003E-2</v>
+        <v>1.3600000000000001E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -5086,7 +5111,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -5124,19 +5149,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -5163,19 +5188,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -5202,19 +5227,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -5241,19 +5266,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -5280,19 +5305,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -5331,20 +5356,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="103.54296875" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="103.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -5405,7 +5430,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.10820000000000002</v>
+        <v>7.3700000000000015E-2</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -5476,11 +5501,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -5514,11 +5539,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.28999999999999998</v>
+        <v>-0.44</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-4.9300000000000004E-2</v>
+        <v>-7.4800000000000005E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -5972,7 +5997,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -6010,19 +6035,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -6049,19 +6074,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -6088,19 +6113,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -6127,19 +6152,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -6166,19 +6191,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -6217,20 +6242,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="103.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="103.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -6291,7 +6316,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.22880000000000006</v>
+        <v>0.31330000000000008</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -6362,11 +6387,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -6400,11 +6425,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.16</v>
+        <v>0.39</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-2.7200000000000002E-2</v>
+        <v>6.6300000000000012E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -6858,7 +6883,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -6896,19 +6921,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -6935,19 +6960,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -6974,19 +6999,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -7013,19 +7038,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -7052,19 +7077,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -7103,20 +7128,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="5" max="5" width="99.6328125" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="17" width="8.81640625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="99.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -7177,7 +7202,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.17590000000000003</v>
+        <v>0.18050000000000002</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -7248,11 +7273,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -7286,11 +7311,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>5.4400000000000004E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -7744,7 +7769,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -7782,19 +7807,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="3">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -7821,19 +7846,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -7860,19 +7885,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -7899,19 +7924,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -7938,19 +7963,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -7988,21 +8013,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="5" max="5" width="100.81640625" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="17" width="8.81640625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="100.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -8063,7 +8088,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.22690000000000005</v>
+        <v>0.23490000000000003</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -8134,11 +8159,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -8172,11 +8197,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.37</v>
+        <v>0.47</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>6.2899999999999998E-2</v>
+        <v>7.9899999999999999E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -8630,7 +8655,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -8668,19 +8693,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="3">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -8707,19 +8732,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -8746,19 +8771,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -8785,19 +8810,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -8824,19 +8849,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -8878,20 +8903,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="5" max="5" width="98.90625" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="17" width="8.81640625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="98.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -8952,7 +8977,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.58350000000000013</v>
+        <v>0.31100000000000005</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -9023,11 +9048,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -9061,11 +9086,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.85</v>
+        <v>-0.7</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>0.14450000000000002</v>
+        <v>-0.11899999999999999</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -9519,7 +9544,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -9557,19 +9582,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="3">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -9596,19 +9621,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -9635,19 +9660,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -9674,19 +9699,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -9713,19 +9738,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -9763,21 +9788,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="5" max="5" width="126.90625" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="17" width="8.81640625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="126.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -9838,7 +9863,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.36870000000000003</v>
+        <v>0.26450000000000001</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -9909,11 +9934,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -9947,11 +9972,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.19</v>
+        <v>-0.75</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-3.2300000000000002E-2</v>
+        <v>-0.1275</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -10405,7 +10430,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -10443,19 +10468,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="3">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -10482,19 +10507,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -10521,19 +10546,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -10560,19 +10585,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -10599,19 +10624,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -10650,20 +10675,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="95.1796875" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" customWidth="1"/>
-    <col min="8" max="17" width="7.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="95.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="17" width="7.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -10724,7 +10749,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.25135000000000002</v>
+        <v>8.9350000000000013E-2</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -10795,11 +10820,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -10833,11 +10858,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.57999999999999996</v>
+        <v>-0.32</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>9.8600000000000007E-2</v>
+        <v>-5.4400000000000004E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -11291,7 +11316,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -11329,19 +11354,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -11368,19 +11393,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -11407,19 +11432,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -11446,19 +11471,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -11485,19 +11510,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -11536,20 +11561,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
     <col min="5" max="5" width="95" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" customWidth="1"/>
-    <col min="8" max="17" width="7.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="17" width="7.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -11610,7 +11635,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.34050000000000008</v>
+        <v>0.22440000000000004</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -11681,11 +11706,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -11719,11 +11744,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.05</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>8.5000000000000006E-3</v>
+        <v>-9.8600000000000007E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -12177,7 +12202,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -12215,19 +12240,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -12254,19 +12279,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -12293,19 +12318,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -12332,19 +12357,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -12371,19 +12396,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -12422,20 +12447,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="101.81640625" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" customWidth="1"/>
-    <col min="8" max="17" width="7.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="101.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="17" width="7.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -12496,7 +12521,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.32469999999999999</v>
+        <v>0.33099999999999996</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -12567,11 +12592,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -12605,11 +12630,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.74</v>
+        <v>-0.65</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-0.1258</v>
+        <v>-0.11050000000000001</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -13063,7 +13088,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -13101,19 +13126,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -13140,19 +13165,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -13179,19 +13204,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -13218,19 +13243,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -13257,19 +13282,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -13308,20 +13333,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="102.7265625" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="102.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -13382,7 +13407,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.55725000000000002</v>
+        <v>0.28475000000000006</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -13453,11 +13478,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -13491,11 +13516,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.85</v>
+        <v>-0.7</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>0.14450000000000002</v>
+        <v>-0.11899999999999999</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -13949,7 +13974,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -13987,19 +14012,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -14026,19 +14051,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -14065,19 +14090,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -14104,19 +14129,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -14143,19 +14168,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -14194,20 +14219,20 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="98.90625" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="98.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -14268,7 +14293,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.23300000000000004</v>
+        <v>0.31240000000000001</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -14339,11 +14364,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>9.0000000000000011E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -14377,11 +14402,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.7</v>
+        <v>-0.18</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>-0.11899999999999999</v>
+        <v>-3.0600000000000002E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -14835,7 +14860,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -14873,19 +14898,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.5</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.1</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -14912,19 +14937,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -14951,19 +14976,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -14990,19 +15015,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -15029,19 +15054,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -15166,20 +15191,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="88.54296875" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="88.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -15240,7 +15265,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.52310000000000001</v>
+        <v>0.28250000000000003</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -15311,11 +15336,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>0.1125</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -15349,11 +15374,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.53</v>
+        <v>-0.7</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>9.0100000000000013E-2</v>
+        <v>-0.11899999999999999</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -15807,7 +15832,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -15845,19 +15870,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.2</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -15884,19 +15909,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -15923,19 +15948,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -15962,19 +15987,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -16001,19 +16026,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -16052,20 +16077,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="98.36328125" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -16126,7 +16151,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.46539999999999998</v>
+        <v>0.47470000000000001</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -16197,11 +16222,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>0.1125</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -16235,11 +16260,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.02</v>
+        <v>0.26</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>3.4000000000000002E-3</v>
+        <v>4.4200000000000003E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -16693,7 +16718,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -16731,19 +16756,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.2</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -16770,19 +16795,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -16809,19 +16834,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -16848,19 +16873,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -16887,19 +16912,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>
@@ -16938,20 +16963,20 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="C24" sqref="C20:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="98.36328125" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="26" width="16.7265625" customWidth="1"/>
-    <col min="27" max="1025" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="1025" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -17012,7 +17037,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.45039999999999997</v>
+        <v>0.22</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -17083,11 +17108,11 @@
       </c>
       <c r="C4" s="1">
         <f>SUM(D20:D24)</f>
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="1">
         <f>B4*C4</f>
-        <v>0.1125</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -17121,11 +17146,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.17</v>
+        <v>-1</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">B5*C5</f>
-        <v>2.8900000000000006E-2</v>
+        <v>-0.17</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -17579,7 +17604,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -17617,19 +17642,19 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
+      <c r="C20" s="18">
+        <v>0.88</v>
       </c>
       <c r="D20" s="1">
         <f>B20*C20</f>
-        <v>0.2</v>
+        <v>0.17600000000000002</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -17656,19 +17681,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C21" s="1">
-        <v>-0.5</v>
+      <c r="C21" s="18">
+        <v>-0.72</v>
       </c>
       <c r="D21" s="1">
         <f>B21*C21</f>
-        <v>-0.1</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -17695,19 +17720,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C22" s="1">
-        <v>0.5</v>
+      <c r="C22" s="18">
+        <v>0.72</v>
       </c>
       <c r="D22" s="1">
         <f>B22*C22</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>22</v>
@@ -17734,19 +17759,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0.2</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.5</v>
+      <c r="C23" s="18">
+        <v>0.72</v>
       </c>
       <c r="D23" s="1">
         <f>B23*C23</f>
-        <v>0.1</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -17773,19 +17798,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
+      <c r="C24" s="18">
+        <v>0.2</v>
       </c>
       <c r="D24" s="1">
         <f>B24*C24</f>
-        <v>0.2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>28</v>

</xml_diff>